<commit_message>
Add loss functions for ZID model
</commit_message>
<xml_diff>
--- a/bin/enhance/data.xlsx
+++ b/bin/enhance/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/data 1/10-workspace/11-code/mon/bin/enhance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/longpham/10-workspace/11-code/mon/bin/enhance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{996C8833-8B22-014C-B8A0-FCF9C6F737B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADDFA7B-2EF0-9040-96BF-E661D7897619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29500" yWindow="500" windowWidth="21620" windowHeight="19880" xr2:uid="{179D6402-3DBB-F649-9704-D7B46CDCA7F1}"/>
+    <workbookView xWindow="25060" yWindow="500" windowWidth="26060" windowHeight="19880" xr2:uid="{179D6402-3DBB-F649-9704-D7B46CDCA7F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Method" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="157">
   <si>
     <t>Method</t>
   </si>
@@ -454,6 +454,60 @@
   </si>
   <si>
     <t>image-size=256 / image-size=256</t>
+  </si>
+  <si>
+    <t>GCENetv2-0110</t>
+  </si>
+  <si>
+    <t>GCENetv2-0111</t>
+  </si>
+  <si>
+    <t>GCENetv2-0112</t>
+  </si>
+  <si>
+    <t>GCENetv2-0113</t>
+  </si>
+  <si>
+    <t>GCENetv2-0114</t>
+  </si>
+  <si>
+    <t>GCENetv2-0115</t>
+  </si>
+  <si>
+    <t>GCENetv2-0120</t>
+  </si>
+  <si>
+    <t>GCENetv2-0121</t>
+  </si>
+  <si>
+    <t>GCENetv2-0122</t>
+  </si>
+  <si>
+    <t>GCENetv2-0123</t>
+  </si>
+  <si>
+    <t>GCENetv2-0124</t>
+  </si>
+  <si>
+    <t>GCENetv2-0125</t>
+  </si>
+  <si>
+    <t>GCENetv2-0130</t>
+  </si>
+  <si>
+    <t>GCENetv2-0131</t>
+  </si>
+  <si>
+    <t>GCENetv2-0132</t>
+  </si>
+  <si>
+    <t>GCENetv2-0133</t>
+  </si>
+  <si>
+    <t>GCENetv2-0134</t>
+  </si>
+  <si>
+    <t>GCENetv2-0135</t>
   </si>
 </sst>
 </file>
@@ -1063,13 +1117,13 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1077,7 +1131,125 @@
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
@@ -1380,65 +1552,79 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1BE7C777-7391-BA49-A2AE-7182DBC1C9B1}" name="Table1" displayName="Table1" ref="A4:B29" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{1BE7C777-7391-BA49-A2AE-7182DBC1C9B1}" name="Table1" displayName="Table1" ref="A4:B29" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="A4:B29" xr:uid="{1BE7C777-7391-BA49-A2AE-7182DBC1C9B1}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:B29">
     <sortCondition ref="B4:B29"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0EDAE7E2-D5FD-224D-9809-955582DE279F}" name="Method" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{CFE0A366-96E3-A848-A2A3-375F1A345F0B}" name="Category" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{0EDAE7E2-D5FD-224D-9809-955582DE279F}" name="Method" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{CFE0A366-96E3-A848-A2A3-375F1A345F0B}" name="Category" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{826EC2C2-36C3-7645-B7DA-02C606F6474F}" name="Table19" displayName="Table19" ref="A31:B81" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{826EC2C2-36C3-7645-B7DA-02C606F6474F}" name="Table19" displayName="Table19" ref="A31:B81" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" tableBorderDxfId="23">
   <autoFilter ref="A31:B81" xr:uid="{826EC2C2-36C3-7645-B7DA-02C606F6474F}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A32:B81">
     <sortCondition ref="A31:A81"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{ACFE5108-46B3-7848-A390-3FA28D58F51B}" name="Method" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{3BC995BA-6262-B247-8D73-E8BA3C59FF7F}" name="Category" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{ACFE5108-46B3-7848-A390-3FA28D58F51B}" name="Method" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{3BC995BA-6262-B247-8D73-E8BA3C59FF7F}" name="Category" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{C68F4D42-EDA1-174E-9121-4DE8279DC1CE}" name="Table1627" displayName="Table1627" ref="A1:Q45" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E155454D-6B5B-ED44-8D23-45C9B66805BA}" name="Table192" displayName="Table192" ref="A83:B133" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" tableBorderDxfId="2">
+  <autoFilter ref="A83:B133" xr:uid="{E155454D-6B5B-ED44-8D23-45C9B66805BA}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A84:B133">
+    <sortCondition ref="A31:A81"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C25E956C-EAF0-B748-8799-09E0DB06381F}" name="Method" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{7B6B519F-6372-B84A-9293-F949DE186C67}" name="Category" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{C68F4D42-EDA1-174E-9121-4DE8279DC1CE}" name="Table1627" displayName="Table1627" ref="A1:Q45" totalsRowShown="0" headerRowDxfId="20">
   <autoFilter ref="A1:Q45" xr:uid="{EDD12726-4FAF-4B4F-B78D-80F569D26274}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F21">
     <sortCondition ref="A1:A21"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{E11CD12C-F780-AD46-8E45-921336810D34}" name="Method" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{1F71EE9C-FEEC-9440-9013-07DD0A019602}" name="Runtime (s)" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{E11CD12C-F780-AD46-8E45-921336810D34}" name="Method" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{1F71EE9C-FEEC-9440-9013-07DD0A019602}" name="Runtime (s)" dataDxfId="18">
       <calculatedColumnFormula>AVERAGE(Table1627[[#This Row],[DCIM]:[VV]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{D41C45A9-67BF-1D4D-8B76-E5EE66850FFD}" name="Frame Rate" dataDxfId="12">
+    <tableColumn id="5" xr3:uid="{D41C45A9-67BF-1D4D-8B76-E5EE66850FFD}" name="Frame Rate" dataDxfId="17">
       <calculatedColumnFormula>1/Table1627[[#This Row],[Runtime (s)]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{EBA33E7B-2A14-914E-9644-CBAA9FA79CF5}" name="Params " dataCellStyle="Comma [0]"/>
-    <tableColumn id="6" xr3:uid="{588EA5A3-2F4F-764D-B48B-509C30BDC356}" name="Params (M)" dataDxfId="11" dataCellStyle="Comma [0]">
+    <tableColumn id="6" xr3:uid="{588EA5A3-2F4F-764D-B48B-509C30BDC356}" name="Params (M)" dataDxfId="16" dataCellStyle="Comma [0]">
       <calculatedColumnFormula>Table1627[[#This Row],[Params ]] * 0.000001</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{AD233B06-3CB1-474C-9980-9608D9E248FB}" name="FLOPs" dataCellStyle="Comma [0]"/>
-    <tableColumn id="7" xr3:uid="{A8841011-9E15-0645-AACE-953E28F21BFF}" name="GFLOPs" dataDxfId="10" dataCellStyle="Comma [0]">
+    <tableColumn id="7" xr3:uid="{A8841011-9E15-0645-AACE-953E28F21BFF}" name="GFLOPs" dataDxfId="15" dataCellStyle="Comma [0]">
       <calculatedColumnFormula>Table1627[[#This Row],[FLOPs]] * 0.000000001</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{DD1FD0EA-2DAE-1D4E-9A5B-CD597B86ED47}" name="DCIM" dataDxfId="9" dataCellStyle="Comma [0]"/>
-    <tableColumn id="19" xr3:uid="{8B60ECB6-4091-C140-A6A2-A1A681BD6DD0}" name="FiveK-E" dataDxfId="8" dataCellStyle="Comma [0]"/>
-    <tableColumn id="9" xr3:uid="{72D5E9D1-8249-FE46-BBB9-E41D44D03D7C}" name="Fusion2" dataDxfId="7" dataCellStyle="Comma [0]"/>
-    <tableColumn id="10" xr3:uid="{86AA2EBD-BAC6-4A44-AAD6-244F48A60934}" name="LIME" dataDxfId="6" dataCellStyle="Comma [0]"/>
-    <tableColumn id="11" xr3:uid="{499692DB-AFE0-4943-AC8D-2406C6613516}" name="LOL-v1" dataDxfId="5" dataCellStyle="Comma [0]"/>
-    <tableColumn id="17" xr3:uid="{2F124F8C-D15C-8041-ABED-3F7ECD448B91}" name="LOL-v2-Real" dataDxfId="4" dataCellStyle="Comma [0]"/>
-    <tableColumn id="18" xr3:uid="{896076E8-A557-834B-9B47-4C2592F55F36}" name="LOL-v2-Syn" dataDxfId="3" dataCellStyle="Comma [0]"/>
-    <tableColumn id="12" xr3:uid="{A4DEF56D-9E2B-3C40-A974-3262F798CEC4}" name="MEF" dataDxfId="2" dataCellStyle="Comma [0]"/>
-    <tableColumn id="13" xr3:uid="{0F5A34E2-F6B6-A34C-907F-EBEF22B6EB21}" name="NPE" dataDxfId="1" dataCellStyle="Comma [0]"/>
-    <tableColumn id="16" xr3:uid="{CCA6180A-2A7D-D144-9AF5-1CC6E936BD43}" name="VV" dataDxfId="0" dataCellStyle="Comma [0]"/>
+    <tableColumn id="8" xr3:uid="{DD1FD0EA-2DAE-1D4E-9A5B-CD597B86ED47}" name="DCIM" dataDxfId="14" dataCellStyle="Comma [0]"/>
+    <tableColumn id="19" xr3:uid="{8B60ECB6-4091-C140-A6A2-A1A681BD6DD0}" name="FiveK-E" dataDxfId="13" dataCellStyle="Comma [0]"/>
+    <tableColumn id="9" xr3:uid="{72D5E9D1-8249-FE46-BBB9-E41D44D03D7C}" name="Fusion2" dataDxfId="12" dataCellStyle="Comma [0]"/>
+    <tableColumn id="10" xr3:uid="{86AA2EBD-BAC6-4A44-AAD6-244F48A60934}" name="LIME" dataDxfId="11" dataCellStyle="Comma [0]"/>
+    <tableColumn id="11" xr3:uid="{499692DB-AFE0-4943-AC8D-2406C6613516}" name="LOL-v1" dataDxfId="10" dataCellStyle="Comma [0]"/>
+    <tableColumn id="17" xr3:uid="{2F124F8C-D15C-8041-ABED-3F7ECD448B91}" name="LOL-v2-Real" dataDxfId="9" dataCellStyle="Comma [0]"/>
+    <tableColumn id="18" xr3:uid="{896076E8-A557-834B-9B47-4C2592F55F36}" name="LOL-v2-Syn" dataDxfId="8" dataCellStyle="Comma [0]"/>
+    <tableColumn id="12" xr3:uid="{A4DEF56D-9E2B-3C40-A974-3262F798CEC4}" name="MEF" dataDxfId="7" dataCellStyle="Comma [0]"/>
+    <tableColumn id="13" xr3:uid="{0F5A34E2-F6B6-A34C-907F-EBEF22B6EB21}" name="NPE" dataDxfId="6" dataCellStyle="Comma [0]"/>
+    <tableColumn id="16" xr3:uid="{CCA6180A-2A7D-D144-9AF5-1CC6E936BD43}" name="VV" dataDxfId="5" dataCellStyle="Comma [0]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1744,13 +1930,13 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:CJ81"/>
+  <dimension ref="A1:CJ133"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="BJ62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I29" sqref="I29:K29"/>
+      <selection pane="bottomRight" activeCell="BQ84" sqref="BQ84:BS84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1811,184 +1997,184 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:88" x14ac:dyDescent="0.2">
-      <c r="D1" s="114" t="s">
+      <c r="D1" s="112" t="s">
         <v>136</v>
       </c>
-      <c r="E1" s="114"/>
-      <c r="F1" s="114"/>
-      <c r="G1" s="114"/>
-      <c r="H1" s="114"/>
-      <c r="I1" s="114"/>
-      <c r="J1" s="114"/>
-      <c r="K1" s="114"/>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
-      <c r="N1" s="114"/>
-      <c r="O1" s="114"/>
-      <c r="Q1" s="114" t="s">
+      <c r="E1" s="112"/>
+      <c r="F1" s="112"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+      <c r="M1" s="112"/>
+      <c r="N1" s="112"/>
+      <c r="O1" s="112"/>
+      <c r="Q1" s="112" t="s">
         <v>53</v>
       </c>
-      <c r="R1" s="114"/>
-      <c r="S1" s="114"/>
-      <c r="T1" s="114"/>
-      <c r="U1" s="114"/>
-      <c r="V1" s="114"/>
-      <c r="W1" s="114"/>
-      <c r="X1" s="114"/>
-      <c r="Z1" s="114" t="s">
+      <c r="R1" s="112"/>
+      <c r="S1" s="112"/>
+      <c r="T1" s="112"/>
+      <c r="U1" s="112"/>
+      <c r="V1" s="112"/>
+      <c r="W1" s="112"/>
+      <c r="X1" s="112"/>
+      <c r="Z1" s="112" t="s">
         <v>49</v>
       </c>
-      <c r="AA1" s="114"/>
-      <c r="AB1" s="114"/>
-      <c r="AC1" s="114"/>
-      <c r="AD1" s="114"/>
-      <c r="AE1" s="114"/>
-      <c r="AF1" s="114"/>
-      <c r="AG1" s="114"/>
-      <c r="AI1" s="114" t="s">
+      <c r="AA1" s="112"/>
+      <c r="AB1" s="112"/>
+      <c r="AC1" s="112"/>
+      <c r="AD1" s="112"/>
+      <c r="AE1" s="112"/>
+      <c r="AF1" s="112"/>
+      <c r="AG1" s="112"/>
+      <c r="AI1" s="112" t="s">
         <v>50</v>
       </c>
-      <c r="AJ1" s="114"/>
-      <c r="AK1" s="114"/>
-      <c r="AL1" s="114"/>
-      <c r="AM1" s="114"/>
-      <c r="AN1" s="114"/>
-      <c r="AO1" s="114"/>
-      <c r="AP1" s="114"/>
-      <c r="AR1" s="114" t="s">
+      <c r="AJ1" s="112"/>
+      <c r="AK1" s="112"/>
+      <c r="AL1" s="112"/>
+      <c r="AM1" s="112"/>
+      <c r="AN1" s="112"/>
+      <c r="AO1" s="112"/>
+      <c r="AP1" s="112"/>
+      <c r="AR1" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="AS1" s="114"/>
-      <c r="AT1" s="114"/>
-      <c r="AU1" s="114"/>
-      <c r="AV1" s="114"/>
-      <c r="AW1" s="114"/>
-      <c r="AX1" s="114"/>
-      <c r="AY1" s="114"/>
-      <c r="BA1" s="114" t="s">
+      <c r="AS1" s="112"/>
+      <c r="AT1" s="112"/>
+      <c r="AU1" s="112"/>
+      <c r="AV1" s="112"/>
+      <c r="AW1" s="112"/>
+      <c r="AX1" s="112"/>
+      <c r="AY1" s="112"/>
+      <c r="BA1" s="112" t="s">
         <v>79</v>
       </c>
-      <c r="BB1" s="112"/>
-      <c r="BC1" s="112"/>
-      <c r="BE1" s="114" t="s">
+      <c r="BB1" s="113"/>
+      <c r="BC1" s="113"/>
+      <c r="BE1" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="BF1" s="112"/>
-      <c r="BG1" s="112"/>
-      <c r="BI1" s="114" t="s">
+      <c r="BF1" s="113"/>
+      <c r="BG1" s="113"/>
+      <c r="BI1" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="BJ1" s="114"/>
-      <c r="BK1" s="114"/>
-      <c r="BM1" s="114" t="s">
+      <c r="BJ1" s="112"/>
+      <c r="BK1" s="112"/>
+      <c r="BM1" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="BN1" s="112"/>
-      <c r="BO1" s="112"/>
-      <c r="BQ1" s="114" t="s">
+      <c r="BN1" s="113"/>
+      <c r="BO1" s="113"/>
+      <c r="BQ1" s="112" t="s">
         <v>9</v>
       </c>
-      <c r="BR1" s="112"/>
-      <c r="BS1" s="112"/>
-      <c r="BU1" s="112" t="s">
+      <c r="BR1" s="113"/>
+      <c r="BS1" s="113"/>
+      <c r="BU1" s="113" t="s">
         <v>119</v>
       </c>
-      <c r="BV1" s="112"/>
-      <c r="BW1" s="112"/>
-      <c r="BX1" s="112"/>
-      <c r="BY1" s="112"/>
-      <c r="BZ1" s="112"/>
-      <c r="CA1" s="112"/>
-      <c r="CB1" s="112"/>
-      <c r="CC1" s="112"/>
-      <c r="CD1" s="112"/>
-      <c r="CE1" s="112"/>
-      <c r="CF1" s="112"/>
-      <c r="CG1" s="112"/>
-      <c r="CH1" s="112"/>
-      <c r="CI1" s="112"/>
-      <c r="CJ1" s="112"/>
+      <c r="BV1" s="113"/>
+      <c r="BW1" s="113"/>
+      <c r="BX1" s="113"/>
+      <c r="BY1" s="113"/>
+      <c r="BZ1" s="113"/>
+      <c r="CA1" s="113"/>
+      <c r="CB1" s="113"/>
+      <c r="CC1" s="113"/>
+      <c r="CD1" s="113"/>
+      <c r="CE1" s="113"/>
+      <c r="CF1" s="113"/>
+      <c r="CG1" s="113"/>
+      <c r="CH1" s="113"/>
+      <c r="CI1" s="113"/>
+      <c r="CJ1" s="113"/>
     </row>
     <row r="2" spans="1:88" x14ac:dyDescent="0.2">
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="E2" s="112"/>
-      <c r="F2" s="112"/>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
-      <c r="M2" s="112"/>
-      <c r="N2" s="112"/>
-      <c r="O2" s="112"/>
-      <c r="Q2" s="112" t="s">
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
+      <c r="O2" s="113"/>
+      <c r="Q2" s="113" t="s">
         <v>137</v>
       </c>
-      <c r="R2" s="112"/>
-      <c r="S2" s="112"/>
-      <c r="T2" s="112"/>
-      <c r="U2" s="112"/>
-      <c r="V2" s="112"/>
-      <c r="W2" s="112"/>
-      <c r="X2" s="112"/>
-      <c r="Z2" s="112" t="s">
+      <c r="R2" s="113"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="113"/>
+      <c r="U2" s="113"/>
+      <c r="V2" s="113"/>
+      <c r="W2" s="113"/>
+      <c r="X2" s="113"/>
+      <c r="Z2" s="113" t="s">
         <v>137</v>
       </c>
-      <c r="AA2" s="112"/>
-      <c r="AB2" s="112"/>
-      <c r="AC2" s="112"/>
-      <c r="AD2" s="112"/>
-      <c r="AE2" s="112"/>
-      <c r="AF2" s="112"/>
-      <c r="AG2" s="112"/>
-      <c r="AI2" s="112" t="s">
+      <c r="AA2" s="113"/>
+      <c r="AB2" s="113"/>
+      <c r="AC2" s="113"/>
+      <c r="AD2" s="113"/>
+      <c r="AE2" s="113"/>
+      <c r="AF2" s="113"/>
+      <c r="AG2" s="113"/>
+      <c r="AI2" s="113" t="s">
         <v>137</v>
       </c>
-      <c r="AJ2" s="112"/>
-      <c r="AK2" s="112"/>
-      <c r="AL2" s="112"/>
-      <c r="AM2" s="112"/>
-      <c r="AN2" s="112"/>
-      <c r="AO2" s="112"/>
-      <c r="AP2" s="112"/>
-      <c r="AR2" s="112" t="s">
+      <c r="AJ2" s="113"/>
+      <c r="AK2" s="113"/>
+      <c r="AL2" s="113"/>
+      <c r="AM2" s="113"/>
+      <c r="AN2" s="113"/>
+      <c r="AO2" s="113"/>
+      <c r="AP2" s="113"/>
+      <c r="AR2" s="113" t="s">
         <v>137</v>
       </c>
-      <c r="AS2" s="112"/>
-      <c r="AT2" s="112"/>
-      <c r="AU2" s="112"/>
-      <c r="AV2" s="112"/>
-      <c r="AW2" s="112"/>
-      <c r="AX2" s="112"/>
-      <c r="AY2" s="112"/>
-      <c r="BA2" s="112" t="s">
+      <c r="AS2" s="113"/>
+      <c r="AT2" s="113"/>
+      <c r="AU2" s="113"/>
+      <c r="AV2" s="113"/>
+      <c r="AW2" s="113"/>
+      <c r="AX2" s="113"/>
+      <c r="AY2" s="113"/>
+      <c r="BA2" s="113" t="s">
         <v>137</v>
       </c>
-      <c r="BB2" s="112"/>
-      <c r="BC2" s="112"/>
-      <c r="BE2" s="112" t="s">
+      <c r="BB2" s="113"/>
+      <c r="BC2" s="113"/>
+      <c r="BE2" s="113" t="s">
         <v>137</v>
       </c>
-      <c r="BF2" s="112"/>
-      <c r="BG2" s="112"/>
-      <c r="BI2" s="112" t="s">
+      <c r="BF2" s="113"/>
+      <c r="BG2" s="113"/>
+      <c r="BI2" s="113" t="s">
         <v>137</v>
       </c>
-      <c r="BJ2" s="112"/>
-      <c r="BK2" s="112"/>
-      <c r="BM2" s="112" t="s">
+      <c r="BJ2" s="113"/>
+      <c r="BK2" s="113"/>
+      <c r="BM2" s="113" t="s">
         <v>137</v>
       </c>
-      <c r="BN2" s="112"/>
-      <c r="BO2" s="112"/>
-      <c r="BQ2" s="112" t="s">
+      <c r="BN2" s="113"/>
+      <c r="BO2" s="113"/>
+      <c r="BQ2" s="113" t="s">
         <v>137</v>
       </c>
-      <c r="BR2" s="112"/>
-      <c r="BS2" s="112"/>
+      <c r="BR2" s="113"/>
+      <c r="BS2" s="113"/>
       <c r="BU2" s="86"/>
       <c r="BV2" s="86"/>
       <c r="BW2" s="86"/>
@@ -2015,14 +2201,14 @@
       <c r="I3" s="108"/>
       <c r="J3" s="108"/>
       <c r="K3" s="108"/>
-      <c r="L3" s="113" t="s">
+      <c r="L3" s="114" t="s">
         <v>131</v>
       </c>
-      <c r="M3" s="113"/>
-      <c r="N3" s="113" t="s">
+      <c r="M3" s="114"/>
+      <c r="N3" s="114" t="s">
         <v>133</v>
       </c>
-      <c r="O3" s="113"/>
+      <c r="O3" s="114"/>
       <c r="Q3" s="109"/>
       <c r="R3" s="109"/>
       <c r="S3" s="109"/>
@@ -13383,19 +13569,427 @@
         <v>3.0300568213000001</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A81" s="67"/>
       <c r="B81" s="67"/>
     </row>
+    <row r="83" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A83" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="B83" s="66" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="84" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A84" s="67" t="s">
+        <v>139</v>
+      </c>
+      <c r="B84" s="67" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z84" s="85">
+        <v>13.165054893500001</v>
+      </c>
+      <c r="AA84" s="86">
+        <v>13.5335769653</v>
+      </c>
+      <c r="AB84" s="86">
+        <v>0.61728143690000004</v>
+      </c>
+      <c r="AC84" s="86">
+        <v>0.82705548600000001</v>
+      </c>
+      <c r="AD84" s="86">
+        <v>0.38949210350000002</v>
+      </c>
+      <c r="AE84" s="86">
+        <v>25.532606124899999</v>
+      </c>
+      <c r="AF84" s="86">
+        <v>7.8573255359000003</v>
+      </c>
+      <c r="AG84" s="87">
+        <v>4.5764418182000002</v>
+      </c>
+      <c r="AI84" s="85">
+        <v>16.126486720999999</v>
+      </c>
+      <c r="AJ84" s="86">
+        <v>16.494518280000001</v>
+      </c>
+      <c r="AK84" s="86">
+        <v>0.65296268459999995</v>
+      </c>
+      <c r="AL84" s="86">
+        <v>0.85620681229999995</v>
+      </c>
+      <c r="AM84" s="86">
+        <v>0.35038490620000001</v>
+      </c>
+      <c r="AN84" s="86">
+        <v>33.430946350100001</v>
+      </c>
+      <c r="AO84" s="86">
+        <v>8.0446136985999992</v>
+      </c>
+      <c r="AP84" s="87">
+        <v>4.6249630802999997</v>
+      </c>
+      <c r="AR84" s="85">
+        <v>16.442269191699999</v>
+      </c>
+      <c r="AS84" s="86">
+        <v>16.760980606099999</v>
+      </c>
+      <c r="AT84" s="86">
+        <v>0.80955761670000004</v>
+      </c>
+      <c r="AU84" s="86">
+        <v>0.88956778169999995</v>
+      </c>
+      <c r="AV84" s="86">
+        <v>0.23111222679999999</v>
+      </c>
+      <c r="AW84" s="86">
+        <v>20.294881820699999</v>
+      </c>
+      <c r="AX84" s="86">
+        <v>4.4465003394</v>
+      </c>
+      <c r="AY84" s="87">
+        <v>3.3116510285</v>
+      </c>
+      <c r="BA84" s="85">
+        <v>23.684295654300001</v>
+      </c>
+      <c r="BB84" s="86">
+        <v>3.8933082279</v>
+      </c>
+      <c r="BC84" s="87">
+        <v>3.0250694002</v>
+      </c>
+      <c r="BE84" s="85">
+        <v>18.5216197968</v>
+      </c>
+      <c r="BF84" s="86">
+        <v>3.9133371254</v>
+      </c>
+      <c r="BG84" s="87">
+        <v>2.7983811850999998</v>
+      </c>
+      <c r="BI84" s="85">
+        <v>15.8301172256</v>
+      </c>
+      <c r="BJ84" s="86">
+        <v>3.3636631438000002</v>
+      </c>
+      <c r="BK84" s="87">
+        <v>2.3891468342</v>
+      </c>
+      <c r="BM84" s="85">
+        <v>18.227722168</v>
+      </c>
+      <c r="BN84" s="86">
+        <v>4.234509955</v>
+      </c>
+      <c r="BO84" s="87">
+        <v>2.9604239643999999</v>
+      </c>
+      <c r="BQ84" s="85">
+        <v>24.603231430099999</v>
+      </c>
+      <c r="BR84" s="86">
+        <v>2.6316908507000001</v>
+      </c>
+      <c r="BS84" s="87">
+        <v>2.9725582096999998</v>
+      </c>
+    </row>
+    <row r="85" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A85" s="67" t="s">
+        <v>140</v>
+      </c>
+      <c r="B85" s="67" t="s">
+        <v>77</v>
+      </c>
+      <c r="BA85" s="85">
+        <v>21.655567169200001</v>
+      </c>
+      <c r="BB85" s="86">
+        <v>7.0829517824000003</v>
+      </c>
+      <c r="BC85" s="87">
+        <v>4.2775363108000004</v>
+      </c>
+      <c r="BE85" s="85">
+        <v>22.863513946499999</v>
+      </c>
+      <c r="BF85" s="86">
+        <v>7.1896409484000001</v>
+      </c>
+      <c r="BG85" s="87">
+        <v>4.2546376241999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A86" s="67" t="s">
+        <v>141</v>
+      </c>
+      <c r="B86" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="87" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A87" s="67" t="s">
+        <v>142</v>
+      </c>
+      <c r="B87" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="88" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A88" s="67" t="s">
+        <v>143</v>
+      </c>
+      <c r="B88" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="89" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A89" s="67" t="s">
+        <v>144</v>
+      </c>
+      <c r="B89" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="90" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A90" s="67"/>
+      <c r="B90" s="67"/>
+    </row>
+    <row r="91" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A91" s="67" t="s">
+        <v>145</v>
+      </c>
+      <c r="B91" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="92" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A92" s="67" t="s">
+        <v>146</v>
+      </c>
+      <c r="B92" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="93" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A93" s="67" t="s">
+        <v>147</v>
+      </c>
+      <c r="B93" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="94" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A94" s="67" t="s">
+        <v>148</v>
+      </c>
+      <c r="B94" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="95" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A95" s="67" t="s">
+        <v>149</v>
+      </c>
+      <c r="B95" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="96" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A96" s="67" t="s">
+        <v>150</v>
+      </c>
+      <c r="B96" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A97" s="67"/>
+      <c r="B97" s="67"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A98" s="67" t="s">
+        <v>151</v>
+      </c>
+      <c r="B98" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A99" s="67" t="s">
+        <v>152</v>
+      </c>
+      <c r="B99" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A100" s="67" t="s">
+        <v>153</v>
+      </c>
+      <c r="B100" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A101" s="67" t="s">
+        <v>154</v>
+      </c>
+      <c r="B101" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A102" s="67" t="s">
+        <v>155</v>
+      </c>
+      <c r="B102" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A103" s="67" t="s">
+        <v>156</v>
+      </c>
+      <c r="B103" s="67" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A104" s="77"/>
+      <c r="B104" s="67"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A105" s="67"/>
+      <c r="B105" s="67"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A106" s="77"/>
+      <c r="B106" s="67"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A107" s="77"/>
+      <c r="B107" s="67"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A108" s="77"/>
+      <c r="B108" s="67"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A109" s="77"/>
+      <c r="B109" s="67"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A110" s="77"/>
+      <c r="B110" s="67"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A111" s="104"/>
+      <c r="B111" s="67"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A112" s="77"/>
+      <c r="B112" s="67"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A113" s="77"/>
+      <c r="B113" s="67"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A114" s="67"/>
+      <c r="B114" s="67"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A115" s="105"/>
+      <c r="B115" s="67"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A116" s="105"/>
+      <c r="B116" s="67"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" s="105"/>
+      <c r="B117" s="67"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" s="106"/>
+      <c r="B118" s="67"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" s="106"/>
+      <c r="B119" s="67"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" s="106"/>
+      <c r="B120" s="67"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" s="106"/>
+      <c r="B121" s="67"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" s="106"/>
+      <c r="B122" s="67"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" s="106"/>
+      <c r="B123" s="67"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A124" s="67"/>
+      <c r="B124" s="67"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="68"/>
+      <c r="B125" s="67"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="68"/>
+      <c r="B126" s="67"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="68"/>
+      <c r="B127" s="67"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A128" s="69"/>
+      <c r="B128" s="67"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A129" s="69"/>
+      <c r="B129" s="67"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A130" s="69"/>
+      <c r="B130" s="67"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A131" s="69"/>
+      <c r="B131" s="67"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A132" s="69"/>
+      <c r="B132" s="67"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A133" s="67"/>
+      <c r="B133" s="67"/>
+    </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="BI1:BK1"/>
-    <mergeCell ref="BQ2:BS2"/>
-    <mergeCell ref="AR2:AY2"/>
-    <mergeCell ref="BA2:BC2"/>
-    <mergeCell ref="BE2:BG2"/>
-    <mergeCell ref="BI2:BK2"/>
-    <mergeCell ref="BM2:BO2"/>
     <mergeCell ref="BU1:CJ1"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="L3:M3"/>
@@ -13412,12 +14006,21 @@
     <mergeCell ref="Q2:X2"/>
     <mergeCell ref="BA1:BC1"/>
     <mergeCell ref="BE1:BG1"/>
+    <mergeCell ref="BI1:BK1"/>
+    <mergeCell ref="BQ2:BS2"/>
+    <mergeCell ref="AR2:AY2"/>
+    <mergeCell ref="BA2:BC2"/>
+    <mergeCell ref="BE2:BG2"/>
+    <mergeCell ref="BI2:BK2"/>
+    <mergeCell ref="BM2:BO2"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <tableParts count="2">
+  <tableParts count="3">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Improve the evaluation pipeline for better logging display
</commit_message>
<xml_diff>
--- a/bin/enhance/data.xlsx
+++ b/bin/enhance/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/longpham/10-workspace/11-code/mon/bin/enhance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/data 1/10-workspace/11-code/mon/bin/enhance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADDFA7B-2EF0-9040-96BF-E661D7897619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88BE095A-67CF-4B4B-8CEB-E1540D31AE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25060" yWindow="500" windowWidth="26060" windowHeight="19880" xr2:uid="{179D6402-3DBB-F649-9704-D7B46CDCA7F1}"/>
+    <workbookView xWindow="25120" yWindow="500" windowWidth="26060" windowHeight="19880" xr2:uid="{179D6402-3DBB-F649-9704-D7B46CDCA7F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Method" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="193">
   <si>
     <t>Method</t>
   </si>
@@ -508,6 +508,114 @@
   </si>
   <si>
     <t>GCENetv2-0135</t>
+  </si>
+  <si>
+    <t>GCENetv2-0140</t>
+  </si>
+  <si>
+    <t>GCENetv2-0141</t>
+  </si>
+  <si>
+    <t>GCENetv2-0142</t>
+  </si>
+  <si>
+    <t>GCENetv2-0143</t>
+  </si>
+  <si>
+    <t>GCENetv2-0144</t>
+  </si>
+  <si>
+    <t>GCENetv2-0145</t>
+  </si>
+  <si>
+    <t>GCENetv2-0150</t>
+  </si>
+  <si>
+    <t>GCENetv2-0151</t>
+  </si>
+  <si>
+    <t>GCENetv2-0152</t>
+  </si>
+  <si>
+    <t>GCENetv2-0153</t>
+  </si>
+  <si>
+    <t>GCENetv2-0154</t>
+  </si>
+  <si>
+    <t>GCENetv2-0155</t>
+  </si>
+  <si>
+    <t>GCENetv2-0160</t>
+  </si>
+  <si>
+    <t>GCENetv2-0161</t>
+  </si>
+  <si>
+    <t>GCENetv2-0162</t>
+  </si>
+  <si>
+    <t>GCENetv2-0163</t>
+  </si>
+  <si>
+    <t>GCENetv2-0164</t>
+  </si>
+  <si>
+    <t>GCENetv2-0165</t>
+  </si>
+  <si>
+    <t>GCENetv2-0170</t>
+  </si>
+  <si>
+    <t>GCENetv2-0171</t>
+  </si>
+  <si>
+    <t>GCENetv2-0172</t>
+  </si>
+  <si>
+    <t>GCENetv2-0173</t>
+  </si>
+  <si>
+    <t>GCENetv2-0174</t>
+  </si>
+  <si>
+    <t>GCENetv2-0175</t>
+  </si>
+  <si>
+    <t>GCENetv2-0180</t>
+  </si>
+  <si>
+    <t>GCENetv2-0181</t>
+  </si>
+  <si>
+    <t>GCENetv2-0182</t>
+  </si>
+  <si>
+    <t>GCENetv2-0183</t>
+  </si>
+  <si>
+    <t>GCENetv2-0184</t>
+  </si>
+  <si>
+    <t>GCENetv2-0185</t>
+  </si>
+  <si>
+    <t>GCENetv2-0190</t>
+  </si>
+  <si>
+    <t>GCENetv2-0191</t>
+  </si>
+  <si>
+    <t>GCENetv2-0192</t>
+  </si>
+  <si>
+    <t>GCENetv2-0193</t>
+  </si>
+  <si>
+    <t>GCENetv2-0194</t>
+  </si>
+  <si>
+    <t>GCENetv2-0195</t>
   </si>
 </sst>
 </file>
@@ -874,7 +982,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1126,130 +1234,15 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="30">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="5"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="5"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4"/>
-        </left>
-        <right style="thin">
-          <color theme="4"/>
-        </right>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="5"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
@@ -1522,6 +1515,124 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="5"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1580,51 +1691,51 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E155454D-6B5B-ED44-8D23-45C9B66805BA}" name="Table192" displayName="Table192" ref="A83:B133" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" tableBorderDxfId="2">
-  <autoFilter ref="A83:B133" xr:uid="{E155454D-6B5B-ED44-8D23-45C9B66805BA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E155454D-6B5B-ED44-8D23-45C9B66805BA}" name="Table192" displayName="Table192" ref="A83:B146" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
+  <autoFilter ref="A83:B146" xr:uid="{E155454D-6B5B-ED44-8D23-45C9B66805BA}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A84:B133">
     <sortCondition ref="A31:A81"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C25E956C-EAF0-B748-8799-09E0DB06381F}" name="Method" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{7B6B519F-6372-B84A-9293-F949DE186C67}" name="Category" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C25E956C-EAF0-B748-8799-09E0DB06381F}" name="Method" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{7B6B519F-6372-B84A-9293-F949DE186C67}" name="Category" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{C68F4D42-EDA1-174E-9121-4DE8279DC1CE}" name="Table1627" displayName="Table1627" ref="A1:Q45" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="26" xr:uid="{C68F4D42-EDA1-174E-9121-4DE8279DC1CE}" name="Table1627" displayName="Table1627" ref="A1:Q45" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="A1:Q45" xr:uid="{EDD12726-4FAF-4B4F-B78D-80F569D26274}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F21">
     <sortCondition ref="A1:A21"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{E11CD12C-F780-AD46-8E45-921336810D34}" name="Method" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{1F71EE9C-FEEC-9440-9013-07DD0A019602}" name="Runtime (s)" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{E11CD12C-F780-AD46-8E45-921336810D34}" name="Method" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{1F71EE9C-FEEC-9440-9013-07DD0A019602}" name="Runtime (s)" dataDxfId="13">
       <calculatedColumnFormula>AVERAGE(Table1627[[#This Row],[DCIM]:[VV]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{D41C45A9-67BF-1D4D-8B76-E5EE66850FFD}" name="Frame Rate" dataDxfId="17">
+    <tableColumn id="5" xr3:uid="{D41C45A9-67BF-1D4D-8B76-E5EE66850FFD}" name="Frame Rate" dataDxfId="12">
       <calculatedColumnFormula>1/Table1627[[#This Row],[Runtime (s)]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{EBA33E7B-2A14-914E-9644-CBAA9FA79CF5}" name="Params " dataCellStyle="Comma [0]"/>
-    <tableColumn id="6" xr3:uid="{588EA5A3-2F4F-764D-B48B-509C30BDC356}" name="Params (M)" dataDxfId="16" dataCellStyle="Comma [0]">
+    <tableColumn id="6" xr3:uid="{588EA5A3-2F4F-764D-B48B-509C30BDC356}" name="Params (M)" dataDxfId="11" dataCellStyle="Comma [0]">
       <calculatedColumnFormula>Table1627[[#This Row],[Params ]] * 0.000001</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{AD233B06-3CB1-474C-9980-9608D9E248FB}" name="FLOPs" dataCellStyle="Comma [0]"/>
-    <tableColumn id="7" xr3:uid="{A8841011-9E15-0645-AACE-953E28F21BFF}" name="GFLOPs" dataDxfId="15" dataCellStyle="Comma [0]">
+    <tableColumn id="7" xr3:uid="{A8841011-9E15-0645-AACE-953E28F21BFF}" name="GFLOPs" dataDxfId="10" dataCellStyle="Comma [0]">
       <calculatedColumnFormula>Table1627[[#This Row],[FLOPs]] * 0.000000001</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{DD1FD0EA-2DAE-1D4E-9A5B-CD597B86ED47}" name="DCIM" dataDxfId="14" dataCellStyle="Comma [0]"/>
-    <tableColumn id="19" xr3:uid="{8B60ECB6-4091-C140-A6A2-A1A681BD6DD0}" name="FiveK-E" dataDxfId="13" dataCellStyle="Comma [0]"/>
-    <tableColumn id="9" xr3:uid="{72D5E9D1-8249-FE46-BBB9-E41D44D03D7C}" name="Fusion2" dataDxfId="12" dataCellStyle="Comma [0]"/>
-    <tableColumn id="10" xr3:uid="{86AA2EBD-BAC6-4A44-AAD6-244F48A60934}" name="LIME" dataDxfId="11" dataCellStyle="Comma [0]"/>
-    <tableColumn id="11" xr3:uid="{499692DB-AFE0-4943-AC8D-2406C6613516}" name="LOL-v1" dataDxfId="10" dataCellStyle="Comma [0]"/>
-    <tableColumn id="17" xr3:uid="{2F124F8C-D15C-8041-ABED-3F7ECD448B91}" name="LOL-v2-Real" dataDxfId="9" dataCellStyle="Comma [0]"/>
-    <tableColumn id="18" xr3:uid="{896076E8-A557-834B-9B47-4C2592F55F36}" name="LOL-v2-Syn" dataDxfId="8" dataCellStyle="Comma [0]"/>
-    <tableColumn id="12" xr3:uid="{A4DEF56D-9E2B-3C40-A974-3262F798CEC4}" name="MEF" dataDxfId="7" dataCellStyle="Comma [0]"/>
-    <tableColumn id="13" xr3:uid="{0F5A34E2-F6B6-A34C-907F-EBEF22B6EB21}" name="NPE" dataDxfId="6" dataCellStyle="Comma [0]"/>
-    <tableColumn id="16" xr3:uid="{CCA6180A-2A7D-D144-9AF5-1CC6E936BD43}" name="VV" dataDxfId="5" dataCellStyle="Comma [0]"/>
+    <tableColumn id="8" xr3:uid="{DD1FD0EA-2DAE-1D4E-9A5B-CD597B86ED47}" name="DCIM" dataDxfId="9" dataCellStyle="Comma [0]"/>
+    <tableColumn id="19" xr3:uid="{8B60ECB6-4091-C140-A6A2-A1A681BD6DD0}" name="FiveK-E" dataDxfId="8" dataCellStyle="Comma [0]"/>
+    <tableColumn id="9" xr3:uid="{72D5E9D1-8249-FE46-BBB9-E41D44D03D7C}" name="Fusion2" dataDxfId="7" dataCellStyle="Comma [0]"/>
+    <tableColumn id="10" xr3:uid="{86AA2EBD-BAC6-4A44-AAD6-244F48A60934}" name="LIME" dataDxfId="6" dataCellStyle="Comma [0]"/>
+    <tableColumn id="11" xr3:uid="{499692DB-AFE0-4943-AC8D-2406C6613516}" name="LOL-v1" dataDxfId="5" dataCellStyle="Comma [0]"/>
+    <tableColumn id="17" xr3:uid="{2F124F8C-D15C-8041-ABED-3F7ECD448B91}" name="LOL-v2-Real" dataDxfId="4" dataCellStyle="Comma [0]"/>
+    <tableColumn id="18" xr3:uid="{896076E8-A557-834B-9B47-4C2592F55F36}" name="LOL-v2-Syn" dataDxfId="3" dataCellStyle="Comma [0]"/>
+    <tableColumn id="12" xr3:uid="{A4DEF56D-9E2B-3C40-A974-3262F798CEC4}" name="MEF" dataDxfId="2" dataCellStyle="Comma [0]"/>
+    <tableColumn id="13" xr3:uid="{0F5A34E2-F6B6-A34C-907F-EBEF22B6EB21}" name="NPE" dataDxfId="1" dataCellStyle="Comma [0]"/>
+    <tableColumn id="16" xr3:uid="{CCA6180A-2A7D-D144-9AF5-1CC6E936BD43}" name="VV" dataDxfId="0" dataCellStyle="Comma [0]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1930,13 +2041,13 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:CJ133"/>
+  <dimension ref="A1:CJ146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="BJ62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="BK75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="BQ84" sqref="BQ84:BS84"/>
+      <selection pane="bottomRight" activeCell="BQ89" sqref="BQ89:BS89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13589,19 +13700,19 @@
         <v>77</v>
       </c>
       <c r="Z84" s="85">
-        <v>13.165054893500001</v>
+        <v>13.2717569669</v>
       </c>
       <c r="AA84" s="86">
         <v>13.5335769653</v>
       </c>
       <c r="AB84" s="86">
-        <v>0.61728143690000004</v>
+        <v>0.62243301070000001</v>
       </c>
       <c r="AC84" s="86">
-        <v>0.82705548600000001</v>
+        <v>0.8366768201</v>
       </c>
       <c r="AD84" s="86">
-        <v>0.38949210350000002</v>
+        <v>0.26564686300000001</v>
       </c>
       <c r="AE84" s="86">
         <v>25.532606124899999</v>
@@ -13613,7 +13724,7 @@
         <v>4.5764418182000002</v>
       </c>
       <c r="AI84" s="85">
-        <v>16.126486720999999</v>
+        <v>16.346291217800001</v>
       </c>
       <c r="AJ84" s="86">
         <v>16.494518280000001</v>
@@ -13622,10 +13733,10 @@
         <v>0.65296268459999995</v>
       </c>
       <c r="AL84" s="86">
-        <v>0.85620681229999995</v>
+        <v>0.87751767400000003</v>
       </c>
       <c r="AM84" s="86">
-        <v>0.35038490620000001</v>
+        <v>0.25610410350000001</v>
       </c>
       <c r="AN84" s="86">
         <v>33.430946350100001</v>
@@ -13637,7 +13748,7 @@
         <v>4.6249630802999997</v>
       </c>
       <c r="AR84" s="85">
-        <v>16.442269191699999</v>
+        <v>16.5653351212</v>
       </c>
       <c r="AS84" s="86">
         <v>16.760980606099999</v>
@@ -13646,10 +13757,10 @@
         <v>0.80955761670000004</v>
       </c>
       <c r="AU84" s="86">
-        <v>0.88956778169999995</v>
+        <v>0.88972070039999995</v>
       </c>
       <c r="AV84" s="86">
-        <v>0.23111222679999999</v>
+        <v>0.22843598039999999</v>
       </c>
       <c r="AW84" s="86">
         <v>20.294881820699999</v>
@@ -13713,23 +13824,122 @@
       <c r="B85" s="67" t="s">
         <v>77</v>
       </c>
+      <c r="Z85" s="85">
+        <v>12.0180323919</v>
+      </c>
+      <c r="AA85" s="86">
+        <v>12.1663599014</v>
+      </c>
+      <c r="AB85" s="86">
+        <v>0.57399325170000004</v>
+      </c>
+      <c r="AC85" s="86">
+        <v>0.80448875819999999</v>
+      </c>
+      <c r="AD85" s="86">
+        <v>0.24433130820000001</v>
+      </c>
+      <c r="AE85" s="86">
+        <v>21.6557178497</v>
+      </c>
+      <c r="AF85" s="86">
+        <v>7.7450498361999998</v>
+      </c>
+      <c r="AG85" s="87">
+        <v>4.7824762464999999</v>
+      </c>
+      <c r="AI85" s="85">
+        <v>14.999726319300001</v>
+      </c>
+      <c r="AJ85" s="86">
+        <v>14.8109664917</v>
+      </c>
+      <c r="AK85" s="86">
+        <v>0.61427508890000004</v>
+      </c>
+      <c r="AL85" s="86">
+        <v>0.86141258720000002</v>
+      </c>
+      <c r="AM85" s="86">
+        <v>0.22146467080000001</v>
+      </c>
+      <c r="AN85" s="86">
+        <v>30.243947982800002</v>
+      </c>
+      <c r="AO85" s="86">
+        <v>7.9024803355</v>
+      </c>
+      <c r="AP85" s="87">
+        <v>4.6986129777999999</v>
+      </c>
+      <c r="AR85" s="85">
+        <v>16.074072504</v>
+      </c>
+      <c r="AS85" s="86">
+        <v>15.9866952896</v>
+      </c>
+      <c r="AT85" s="86">
+        <v>0.7755056038</v>
+      </c>
+      <c r="AU85" s="86">
+        <v>0.88458484469999998</v>
+      </c>
+      <c r="AV85" s="86">
+        <v>0.21046159410000001</v>
+      </c>
+      <c r="AW85" s="86">
+        <v>19.457773208599999</v>
+      </c>
+      <c r="AX85" s="86">
+        <v>4.4407742237000001</v>
+      </c>
+      <c r="AY85" s="87">
+        <v>3.3294495834000002</v>
+      </c>
       <c r="BA85" s="85">
-        <v>21.655567169200001</v>
+        <v>22.3399162292</v>
       </c>
       <c r="BB85" s="86">
-        <v>7.0829517824000003</v>
+        <v>3.8883973233</v>
       </c>
       <c r="BC85" s="87">
-        <v>4.2775363108000004</v>
+        <v>3.0290721430000001</v>
       </c>
       <c r="BE85" s="85">
-        <v>22.863513946499999</v>
+        <v>17.986804962200001</v>
       </c>
       <c r="BF85" s="86">
-        <v>7.1896409484000001</v>
+        <v>3.8984490004999999</v>
       </c>
       <c r="BG85" s="87">
-        <v>4.2546376241999999</v>
+        <v>2.8256081210000001</v>
+      </c>
+      <c r="BI85" s="85">
+        <v>15.4814271927</v>
+      </c>
+      <c r="BJ85" s="86">
+        <v>3.3638647960000001</v>
+      </c>
+      <c r="BK85" s="87">
+        <v>2.4095816860000001</v>
+      </c>
+      <c r="BM85" s="85">
+        <v>18.0598144531</v>
+      </c>
+      <c r="BN85" s="86">
+        <v>4.2037987940999999</v>
+      </c>
+      <c r="BO85" s="87">
+        <v>2.9024239780999999</v>
+      </c>
+      <c r="BQ85" s="85">
+        <v>22.399639129600001</v>
+      </c>
+      <c r="BR85" s="86">
+        <v>2.6693954419999999</v>
+      </c>
+      <c r="BS85" s="87">
+        <v>3.0041651874999999</v>
       </c>
     </row>
     <row r="86" spans="1:71" x14ac:dyDescent="0.2">
@@ -13739,6 +13949,123 @@
       <c r="B86" s="67" t="s">
         <v>77</v>
       </c>
+      <c r="Z86" s="85">
+        <v>11.9889380137</v>
+      </c>
+      <c r="AA86" s="86">
+        <v>12.123558044399999</v>
+      </c>
+      <c r="AB86" s="86">
+        <v>0.57344680429999995</v>
+      </c>
+      <c r="AC86" s="86">
+        <v>0.80458135210000004</v>
+      </c>
+      <c r="AD86" s="86">
+        <v>0.2469003608</v>
+      </c>
+      <c r="AE86" s="86">
+        <v>21.3740119934</v>
+      </c>
+      <c r="AF86" s="86">
+        <v>7.7356941331</v>
+      </c>
+      <c r="AG86" s="87">
+        <v>4.7826624399000002</v>
+      </c>
+      <c r="AI86" s="85">
+        <v>14.947682328200001</v>
+      </c>
+      <c r="AJ86" s="86">
+        <v>14.742789268499999</v>
+      </c>
+      <c r="AK86" s="86">
+        <v>0.61305101390000005</v>
+      </c>
+      <c r="AL86" s="86">
+        <v>0.85954190850000001</v>
+      </c>
+      <c r="AM86" s="86">
+        <v>0.2243502077</v>
+      </c>
+      <c r="AN86" s="86">
+        <v>30.0269966125</v>
+      </c>
+      <c r="AO86" s="86">
+        <v>7.8909161211000001</v>
+      </c>
+      <c r="AP86" s="87">
+        <v>4.7001562368999998</v>
+      </c>
+      <c r="AR86" s="85">
+        <v>15.964799985899999</v>
+      </c>
+      <c r="AS86" s="86">
+        <v>15.863792419399999</v>
+      </c>
+      <c r="AT86" s="86">
+        <v>0.7762982249</v>
+      </c>
+      <c r="AU86" s="86">
+        <v>0.88459163669999996</v>
+      </c>
+      <c r="AV86" s="86">
+        <v>0.21121496940000001</v>
+      </c>
+      <c r="AW86" s="86">
+        <v>19.511991500899999</v>
+      </c>
+      <c r="AX86" s="86">
+        <v>4.4322970240000004</v>
+      </c>
+      <c r="AY86" s="87">
+        <v>3.3174624979999998</v>
+      </c>
+      <c r="BA86" s="85">
+        <v>22.3547935486</v>
+      </c>
+      <c r="BB86" s="86">
+        <v>3.8555062660999999</v>
+      </c>
+      <c r="BC86" s="87">
+        <v>3.0124968255</v>
+      </c>
+      <c r="BE86" s="85">
+        <v>17.999547958400001</v>
+      </c>
+      <c r="BF86" s="86">
+        <v>3.8674298560999998</v>
+      </c>
+      <c r="BG86" s="87">
+        <v>2.792551719</v>
+      </c>
+      <c r="BI86" s="85">
+        <v>15.249206543</v>
+      </c>
+      <c r="BJ86" s="86">
+        <v>3.3527805302</v>
+      </c>
+      <c r="BK86" s="87">
+        <v>2.3894071563999999</v>
+      </c>
+      <c r="BM86" s="85">
+        <v>18.0598144531</v>
+      </c>
+      <c r="BN86" s="86">
+        <v>4.1973746748999998</v>
+      </c>
+      <c r="BO86" s="87">
+        <v>2.9061809104999998</v>
+      </c>
+      <c r="BQ86" s="85">
+        <v>23.005575180099999</v>
+      </c>
+      <c r="BR86" s="86">
+        <v>2.6590985578000002</v>
+      </c>
+      <c r="BS86" s="87">
+        <v>3.0081247439999999</v>
+      </c>
     </row>
     <row r="87" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A87" s="67" t="s">
@@ -13747,6 +14074,123 @@
       <c r="B87" s="67" t="s">
         <v>77</v>
       </c>
+      <c r="Z87" s="85">
+        <v>11.843056106600001</v>
+      </c>
+      <c r="AA87" s="86">
+        <v>12.0591897964</v>
+      </c>
+      <c r="AB87" s="86">
+        <v>0.56546666219999997</v>
+      </c>
+      <c r="AC87" s="86">
+        <v>0.79777610700000001</v>
+      </c>
+      <c r="AD87" s="86">
+        <v>0.2403929571</v>
+      </c>
+      <c r="AE87" s="86">
+        <v>21.3219299316</v>
+      </c>
+      <c r="AF87" s="86">
+        <v>7.7116206894000001</v>
+      </c>
+      <c r="AG87" s="87">
+        <v>4.8072356191000001</v>
+      </c>
+      <c r="AI87" s="85">
+        <v>14.7443935347</v>
+      </c>
+      <c r="AJ87" s="86">
+        <v>14.667526245099999</v>
+      </c>
+      <c r="AK87" s="86">
+        <v>0.60888397689999996</v>
+      </c>
+      <c r="AL87" s="86">
+        <v>0.85510752560000003</v>
+      </c>
+      <c r="AM87" s="86">
+        <v>0.22065998989999999</v>
+      </c>
+      <c r="AN87" s="86">
+        <v>29.8517456055</v>
+      </c>
+      <c r="AO87" s="86">
+        <v>7.8878665266999999</v>
+      </c>
+      <c r="AP87" s="87">
+        <v>4.7134124795999996</v>
+      </c>
+      <c r="AR87" s="85">
+        <v>16.033112039599999</v>
+      </c>
+      <c r="AS87" s="86">
+        <v>15.9499139786</v>
+      </c>
+      <c r="AT87" s="86">
+        <v>0.77141960740000004</v>
+      </c>
+      <c r="AU87" s="86">
+        <v>0.88759500680000003</v>
+      </c>
+      <c r="AV87" s="86">
+        <v>0.21261298219999999</v>
+      </c>
+      <c r="AW87" s="86">
+        <v>19.088834762600001</v>
+      </c>
+      <c r="AX87" s="86">
+        <v>4.4153855412</v>
+      </c>
+      <c r="AY87" s="87">
+        <v>3.3208738490999998</v>
+      </c>
+      <c r="BA87" s="85">
+        <v>22.102001190199999</v>
+      </c>
+      <c r="BB87" s="86">
+        <v>3.8844485145999998</v>
+      </c>
+      <c r="BC87" s="87">
+        <v>3.0238394567000002</v>
+      </c>
+      <c r="BE87" s="85">
+        <v>17.6071662903</v>
+      </c>
+      <c r="BF87" s="86">
+        <v>3.8747653985000001</v>
+      </c>
+      <c r="BG87" s="87">
+        <v>2.8039778886</v>
+      </c>
+      <c r="BI87" s="85">
+        <v>15.384116172800001</v>
+      </c>
+      <c r="BJ87" s="86">
+        <v>3.3718059576999999</v>
+      </c>
+      <c r="BK87" s="87">
+        <v>2.4157339283999999</v>
+      </c>
+      <c r="BM87" s="85">
+        <v>17.460998535200002</v>
+      </c>
+      <c r="BN87" s="86">
+        <v>4.1391708022999998</v>
+      </c>
+      <c r="BO87" s="87">
+        <v>2.8925540439000001</v>
+      </c>
+      <c r="BQ87" s="85">
+        <v>22.162090301500001</v>
+      </c>
+      <c r="BR87" s="86">
+        <v>2.6840095071999999</v>
+      </c>
+      <c r="BS87" s="87">
+        <v>3.0309736678000001</v>
+      </c>
     </row>
     <row r="88" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A88" s="67" t="s">
@@ -13755,6 +14199,123 @@
       <c r="B88" s="67" t="s">
         <v>77</v>
       </c>
+      <c r="Z88" s="85">
+        <v>11.915264829</v>
+      </c>
+      <c r="AA88" s="86">
+        <v>12.028439521799999</v>
+      </c>
+      <c r="AB88" s="86">
+        <v>0.56999279059999997</v>
+      </c>
+      <c r="AC88" s="86">
+        <v>0.79927806459999995</v>
+      </c>
+      <c r="AD88" s="86">
+        <v>0.25152540010000002</v>
+      </c>
+      <c r="AE88" s="86">
+        <v>21.286153793299999</v>
+      </c>
+      <c r="AF88" s="86">
+        <v>7.7344340520000001</v>
+      </c>
+      <c r="AG88" s="87">
+        <v>4.7921969658999997</v>
+      </c>
+      <c r="AI88" s="85">
+        <v>14.8564124489</v>
+      </c>
+      <c r="AJ88" s="86">
+        <v>14.641187667800001</v>
+      </c>
+      <c r="AK88" s="86">
+        <v>0.6103942215</v>
+      </c>
+      <c r="AL88" s="86">
+        <v>0.85667402329999998</v>
+      </c>
+      <c r="AM88" s="86">
+        <v>0.22929208000000001</v>
+      </c>
+      <c r="AN88" s="86">
+        <v>29.947715759299999</v>
+      </c>
+      <c r="AO88" s="86">
+        <v>7.8911780792000004</v>
+      </c>
+      <c r="AP88" s="87">
+        <v>4.7221393130999996</v>
+      </c>
+      <c r="AR88" s="85">
+        <v>15.9395801735</v>
+      </c>
+      <c r="AS88" s="86">
+        <v>15.8789196014</v>
+      </c>
+      <c r="AT88" s="86">
+        <v>0.77117960600000002</v>
+      </c>
+      <c r="AU88" s="86">
+        <v>0.88553124370000003</v>
+      </c>
+      <c r="AV88" s="86">
+        <v>0.22121057290000001</v>
+      </c>
+      <c r="AW88" s="86">
+        <v>19.0983295441</v>
+      </c>
+      <c r="AX88" s="86">
+        <v>4.4233820071999999</v>
+      </c>
+      <c r="AY88" s="87">
+        <v>3.3300808038</v>
+      </c>
+      <c r="BA88" s="85">
+        <v>21.7703895569</v>
+      </c>
+      <c r="BB88" s="86">
+        <v>3.8748930054000001</v>
+      </c>
+      <c r="BC88" s="87">
+        <v>3.0210435388999999</v>
+      </c>
+      <c r="BE88" s="85">
+        <v>18.023962020900001</v>
+      </c>
+      <c r="BF88" s="86">
+        <v>3.8917884308000001</v>
+      </c>
+      <c r="BG88" s="87">
+        <v>2.8215856386999998</v>
+      </c>
+      <c r="BI88" s="85">
+        <v>14.8582086563</v>
+      </c>
+      <c r="BJ88" s="86">
+        <v>3.3567921812999999</v>
+      </c>
+      <c r="BK88" s="87">
+        <v>2.4284650547000002</v>
+      </c>
+      <c r="BM88" s="85">
+        <v>17.6354980469</v>
+      </c>
+      <c r="BN88" s="86">
+        <v>4.1654191319000002</v>
+      </c>
+      <c r="BO88" s="87">
+        <v>2.9029094662000001</v>
+      </c>
+      <c r="BQ88" s="85">
+        <v>22.1788539886</v>
+      </c>
+      <c r="BR88" s="86">
+        <v>2.6831166198999998</v>
+      </c>
+      <c r="BS88" s="87">
+        <v>3.0283455382</v>
+      </c>
     </row>
     <row r="89" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A89" s="67" t="s">
@@ -13763,6 +14324,123 @@
       <c r="B89" s="67" t="s">
         <v>77</v>
       </c>
+      <c r="Z89" s="85">
+        <v>11.8918605487</v>
+      </c>
+      <c r="AA89" s="86">
+        <v>12.0705184937</v>
+      </c>
+      <c r="AB89" s="86">
+        <v>0.56900951070000005</v>
+      </c>
+      <c r="AC89" s="86">
+        <v>0.7953909079</v>
+      </c>
+      <c r="AD89" s="86">
+        <v>0.2444562008</v>
+      </c>
+      <c r="AE89" s="86">
+        <v>21.699239730799999</v>
+      </c>
+      <c r="AF89" s="86">
+        <v>7.7233393015000003</v>
+      </c>
+      <c r="AG89" s="87">
+        <v>4.7828998041000004</v>
+      </c>
+      <c r="AI89" s="85">
+        <v>14.7930631542</v>
+      </c>
+      <c r="AJ89" s="86">
+        <v>14.661392211900001</v>
+      </c>
+      <c r="AK89" s="86">
+        <v>0.60907991289999996</v>
+      </c>
+      <c r="AL89" s="86">
+        <v>0.85339812579999996</v>
+      </c>
+      <c r="AM89" s="86">
+        <v>0.22412335219999999</v>
+      </c>
+      <c r="AN89" s="86">
+        <v>30.087852477999999</v>
+      </c>
+      <c r="AO89" s="86">
+        <v>7.8834555671000004</v>
+      </c>
+      <c r="AP89" s="87">
+        <v>4.7028564334</v>
+      </c>
+      <c r="AR89" s="85">
+        <v>16.016513585999999</v>
+      </c>
+      <c r="AS89" s="86">
+        <v>15.916226387</v>
+      </c>
+      <c r="AT89" s="86">
+        <v>0.77428847550000002</v>
+      </c>
+      <c r="AU89" s="86">
+        <v>0.8847746688</v>
+      </c>
+      <c r="AV89" s="86">
+        <v>0.21309827149999999</v>
+      </c>
+      <c r="AW89" s="86">
+        <v>19.383178710900001</v>
+      </c>
+      <c r="AX89" s="86">
+        <v>4.4278838303999999</v>
+      </c>
+      <c r="AY89" s="87">
+        <v>3.3066181681</v>
+      </c>
+      <c r="BA89" s="85">
+        <v>22.1515388489</v>
+      </c>
+      <c r="BB89" s="86">
+        <v>3.8600779981</v>
+      </c>
+      <c r="BC89" s="87">
+        <v>3.0133480885999999</v>
+      </c>
+      <c r="BE89" s="85">
+        <v>18.036512374899999</v>
+      </c>
+      <c r="BF89" s="86">
+        <v>3.8696295695999998</v>
+      </c>
+      <c r="BG89" s="87">
+        <v>2.8076835774000002</v>
+      </c>
+      <c r="BI89" s="85">
+        <v>15.249379158</v>
+      </c>
+      <c r="BJ89" s="86">
+        <v>3.3400224109000001</v>
+      </c>
+      <c r="BK89" s="87">
+        <v>2.4083415082999999</v>
+      </c>
+      <c r="BM89" s="85">
+        <v>18.009704589799998</v>
+      </c>
+      <c r="BN89" s="86">
+        <v>4.1706689369000003</v>
+      </c>
+      <c r="BO89" s="87">
+        <v>2.9264313499000001</v>
+      </c>
+      <c r="BQ89" s="85">
+        <v>22.6762905121</v>
+      </c>
+      <c r="BR89" s="86">
+        <v>2.6644632526000001</v>
+      </c>
+      <c r="BS89" s="87">
+        <v>3.006844471</v>
+      </c>
     </row>
     <row r="90" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A90" s="67"/>
@@ -13775,6 +14453,123 @@
       <c r="B91" s="67" t="s">
         <v>77</v>
       </c>
+      <c r="Z91" s="85">
+        <v>12.064024766299999</v>
+      </c>
+      <c r="AA91" s="86">
+        <v>12.0967950821</v>
+      </c>
+      <c r="AB91" s="86">
+        <v>0.57704584599999997</v>
+      </c>
+      <c r="AC91" s="86">
+        <v>0.80533165529999995</v>
+      </c>
+      <c r="AD91" s="86">
+        <v>0.26421239569999999</v>
+      </c>
+      <c r="AE91" s="86">
+        <v>21.444194793699999</v>
+      </c>
+      <c r="AF91" s="86">
+        <v>7.7279149135000003</v>
+      </c>
+      <c r="AG91" s="87">
+        <v>4.7907967431999996</v>
+      </c>
+      <c r="AI91" s="85">
+        <v>15.043390255</v>
+      </c>
+      <c r="AJ91" s="86">
+        <v>14.731616020200001</v>
+      </c>
+      <c r="AK91" s="86">
+        <v>0.61609605460000005</v>
+      </c>
+      <c r="AL91" s="86">
+        <v>0.86021510599999995</v>
+      </c>
+      <c r="AM91" s="86">
+        <v>0.2402474651</v>
+      </c>
+      <c r="AN91" s="86">
+        <v>30.0748348236</v>
+      </c>
+      <c r="AO91" s="86">
+        <v>7.8817276233999998</v>
+      </c>
+      <c r="AP91" s="87">
+        <v>4.7109806847</v>
+      </c>
+      <c r="AR91" s="85">
+        <v>15.8850574589</v>
+      </c>
+      <c r="AS91" s="86">
+        <v>15.837848663300001</v>
+      </c>
+      <c r="AT91" s="86">
+        <v>0.77535724640000003</v>
+      </c>
+      <c r="AU91" s="86">
+        <v>0.88169783229999998</v>
+      </c>
+      <c r="AV91" s="86">
+        <v>0.22068708670000001</v>
+      </c>
+      <c r="AW91" s="86">
+        <v>19.416416168200001</v>
+      </c>
+      <c r="AX91" s="86">
+        <v>4.427159982</v>
+      </c>
+      <c r="AY91" s="87">
+        <v>3.3196086002</v>
+      </c>
+      <c r="BA91" s="85">
+        <v>22.052516937299998</v>
+      </c>
+      <c r="BB91" s="86">
+        <v>3.8359943010999999</v>
+      </c>
+      <c r="BC91" s="87">
+        <v>3.0058147930999999</v>
+      </c>
+      <c r="BE91" s="85">
+        <v>17.8614635468</v>
+      </c>
+      <c r="BF91" s="86">
+        <v>3.9009341786</v>
+      </c>
+      <c r="BG91" s="87">
+        <v>2.8150900931999998</v>
+      </c>
+      <c r="BI91" s="85">
+        <v>15.1064271927</v>
+      </c>
+      <c r="BJ91" s="86">
+        <v>3.3626706137000002</v>
+      </c>
+      <c r="BK91" s="87">
+        <v>2.4243268362000001</v>
+      </c>
+      <c r="BM91" s="85">
+        <v>18.0803222656</v>
+      </c>
+      <c r="BN91" s="86">
+        <v>4.1743836740000004</v>
+      </c>
+      <c r="BO91" s="87">
+        <v>2.8899469721000002</v>
+      </c>
+      <c r="BQ91" s="85">
+        <v>22.941183090199999</v>
+      </c>
+      <c r="BR91" s="86">
+        <v>2.6508743766</v>
+      </c>
+      <c r="BS91" s="87">
+        <v>2.9969074074000002</v>
+      </c>
     </row>
     <row r="92" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A92" s="67" t="s">
@@ -13816,19 +14611,136 @@
         <v>77</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A97" s="67"/>
       <c r="B97" s="67"/>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A98" s="67" t="s">
         <v>151</v>
       </c>
       <c r="B98" s="67" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="Z98" s="85">
+        <v>11.7660147667</v>
+      </c>
+      <c r="AA98" s="86">
+        <v>11.9343261719</v>
+      </c>
+      <c r="AB98" s="86">
+        <v>0.56161089939999997</v>
+      </c>
+      <c r="AC98" s="86">
+        <v>0.79476137160000004</v>
+      </c>
+      <c r="AD98" s="86">
+        <v>0.24458203319999999</v>
+      </c>
+      <c r="AE98" s="86">
+        <v>21.153146743800001</v>
+      </c>
+      <c r="AF98" s="86">
+        <v>7.7030302906000001</v>
+      </c>
+      <c r="AG98" s="87">
+        <v>4.8366013813000004</v>
+      </c>
+      <c r="AI98" s="85">
+        <v>14.6470651579</v>
+      </c>
+      <c r="AJ98" s="86">
+        <v>14.512243270900001</v>
+      </c>
+      <c r="AK98" s="86">
+        <v>0.60451030729999999</v>
+      </c>
+      <c r="AL98" s="86">
+        <v>0.85300486620000004</v>
+      </c>
+      <c r="AM98" s="86">
+        <v>0.2227691524</v>
+      </c>
+      <c r="AN98" s="86">
+        <v>29.705688476599999</v>
+      </c>
+      <c r="AO98" s="86">
+        <v>7.8799314872000004</v>
+      </c>
+      <c r="AP98" s="87">
+        <v>4.7374749338999997</v>
+      </c>
+      <c r="AR98" s="85">
+        <v>15.8473262978</v>
+      </c>
+      <c r="AS98" s="86">
+        <v>15.737172126800001</v>
+      </c>
+      <c r="AT98" s="86">
+        <v>0.76851716219999999</v>
+      </c>
+      <c r="AU98" s="86">
+        <v>0.88229973319999999</v>
+      </c>
+      <c r="AV98" s="86">
+        <v>0.2147152739</v>
+      </c>
+      <c r="AW98" s="86">
+        <v>19.1530895233</v>
+      </c>
+      <c r="AX98" s="86">
+        <v>4.4288695700999998</v>
+      </c>
+      <c r="AY98" s="87">
+        <v>3.3306027553000002</v>
+      </c>
+      <c r="BA98" s="85">
+        <v>21.9798164368</v>
+      </c>
+      <c r="BB98" s="86">
+        <v>3.8558145072999999</v>
+      </c>
+      <c r="BC98" s="87">
+        <v>3.0160847813</v>
+      </c>
+      <c r="BE98" s="85">
+        <v>17.944568633999999</v>
+      </c>
+      <c r="BF98" s="86">
+        <v>3.8795783241000001</v>
+      </c>
+      <c r="BG98" s="87">
+        <v>2.8239671354000002</v>
+      </c>
+      <c r="BI98" s="85">
+        <v>15.113291740399999</v>
+      </c>
+      <c r="BJ98" s="86">
+        <v>3.3481723910999999</v>
+      </c>
+      <c r="BK98" s="87">
+        <v>2.4086671758999998</v>
+      </c>
+      <c r="BM98" s="85">
+        <v>17.510681152299998</v>
+      </c>
+      <c r="BN98" s="86">
+        <v>4.1547901802</v>
+      </c>
+      <c r="BO98" s="87">
+        <v>2.8817022544999999</v>
+      </c>
+      <c r="BQ98" s="85">
+        <v>22.047262191800002</v>
+      </c>
+      <c r="BR98" s="86">
+        <v>2.6820779425999999</v>
+      </c>
+      <c r="BS98" s="87">
+        <v>3.0241123922000002</v>
+      </c>
+    </row>
+    <row r="99" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A99" s="67" t="s">
         <v>152</v>
       </c>
@@ -13836,7 +14748,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A100" s="67" t="s">
         <v>153</v>
       </c>
@@ -13844,7 +14756,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A101" s="67" t="s">
         <v>154</v>
       </c>
@@ -13852,7 +14764,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A102" s="67" t="s">
         <v>155</v>
       </c>
@@ -13860,7 +14772,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A103" s="67" t="s">
         <v>156</v>
       </c>
@@ -13868,125 +14780,951 @@
         <v>77</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A104" s="77"/>
       <c r="B104" s="67"/>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="67"/>
+    <row r="105" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A105" s="67" t="s">
+        <v>157</v>
+      </c>
       <c r="B105" s="67"/>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A106" s="77"/>
+      <c r="Z105" s="85">
+        <v>11.7734953562</v>
+      </c>
+      <c r="AA105" s="86">
+        <v>11.9675693512</v>
+      </c>
+      <c r="AB105" s="86">
+        <v>0.56298599240000002</v>
+      </c>
+      <c r="AC105" s="86">
+        <v>0.79231326580000005</v>
+      </c>
+      <c r="AD105" s="86">
+        <v>0.24442330200000001</v>
+      </c>
+      <c r="AE105" s="86">
+        <v>21.251844406099998</v>
+      </c>
+      <c r="AF105" s="86">
+        <v>7.7198760181999999</v>
+      </c>
+      <c r="AG105" s="87">
+        <v>4.8185624886999996</v>
+      </c>
+      <c r="AI105" s="85">
+        <v>14.6287693834</v>
+      </c>
+      <c r="AJ105" s="86">
+        <v>14.531298637400001</v>
+      </c>
+      <c r="AK105" s="86">
+        <v>0.60404387179999997</v>
+      </c>
+      <c r="AL105" s="86">
+        <v>0.84973098749999998</v>
+      </c>
+      <c r="AM105" s="86">
+        <v>0.22664816660000001</v>
+      </c>
+      <c r="AN105" s="86">
+        <v>29.924112319900001</v>
+      </c>
+      <c r="AO105" s="86">
+        <v>7.8829962870000001</v>
+      </c>
+      <c r="AP105" s="87">
+        <v>4.7303086653999999</v>
+      </c>
+      <c r="AR105" s="85">
+        <v>15.905913743999999</v>
+      </c>
+      <c r="AS105" s="86">
+        <v>15.8135967255</v>
+      </c>
+      <c r="AT105" s="86">
+        <v>0.77430391249999997</v>
+      </c>
+      <c r="AU105" s="86">
+        <v>0.88342333500000003</v>
+      </c>
+      <c r="AV105" s="86">
+        <v>0.2174774257</v>
+      </c>
+      <c r="AW105" s="86">
+        <v>19.379867553699999</v>
+      </c>
+      <c r="AX105" s="86">
+        <v>4.4139144465999998</v>
+      </c>
+      <c r="AY105" s="87">
+        <v>3.3154121228000002</v>
+      </c>
+      <c r="BA105" s="85">
+        <v>22.161983490000001</v>
+      </c>
+      <c r="BB105" s="86">
+        <v>3.8352228969</v>
+      </c>
+      <c r="BC105" s="87">
+        <v>3.0047881676000001</v>
+      </c>
+      <c r="BE105" s="85">
+        <v>17.985193252599998</v>
+      </c>
+      <c r="BF105" s="86">
+        <v>3.8743883810000002</v>
+      </c>
+      <c r="BG105" s="87">
+        <v>2.7979066487000002</v>
+      </c>
+      <c r="BI105" s="85">
+        <v>15.4195594788</v>
+      </c>
+      <c r="BJ105" s="86">
+        <v>3.3135703204000002</v>
+      </c>
+      <c r="BK105" s="87">
+        <v>2.4097072732</v>
+      </c>
+      <c r="BM105" s="85">
+        <v>17.509094238300001</v>
+      </c>
+      <c r="BN105" s="86">
+        <v>4.1405511723000004</v>
+      </c>
+      <c r="BO105" s="87">
+        <v>2.8787538145</v>
+      </c>
+      <c r="BQ105" s="85">
+        <v>22.4826660156</v>
+      </c>
+      <c r="BR105" s="86">
+        <v>2.6763070512999998</v>
+      </c>
+      <c r="BS105" s="87">
+        <v>3.021923932</v>
+      </c>
+    </row>
+    <row r="106" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A106" s="67" t="s">
+        <v>158</v>
+      </c>
       <c r="B106" s="67"/>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A107" s="77"/>
+    <row r="107" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A107" s="67" t="s">
+        <v>159</v>
+      </c>
       <c r="B107" s="67"/>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A108" s="77"/>
+    <row r="108" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A108" s="67" t="s">
+        <v>160</v>
+      </c>
       <c r="B108" s="67"/>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A109" s="77"/>
+    <row r="109" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A109" s="67" t="s">
+        <v>161</v>
+      </c>
       <c r="B109" s="67"/>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A110" s="77"/>
+    <row r="110" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A110" s="67" t="s">
+        <v>162</v>
+      </c>
       <c r="B110" s="67"/>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A111" s="104"/>
       <c r="B111" s="67"/>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="77"/>
+    <row r="112" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A112" s="67" t="s">
+        <v>163</v>
+      </c>
       <c r="B112" s="67"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A113" s="77"/>
+      <c r="Z112" s="85">
+        <v>11.9097730001</v>
+      </c>
+      <c r="AA112" s="86">
+        <v>12.061985015899999</v>
+      </c>
+      <c r="AB112" s="86">
+        <v>0.57002672350000005</v>
+      </c>
+      <c r="AC112" s="86">
+        <v>0.79496239820000003</v>
+      </c>
+      <c r="AD112" s="86">
+        <v>0.2462263505</v>
+      </c>
+      <c r="AE112" s="86">
+        <v>21.710372924800001</v>
+      </c>
+      <c r="AF112" s="86">
+        <v>7.7658710015999999</v>
+      </c>
+      <c r="AG112" s="87">
+        <v>4.7881203885000003</v>
+      </c>
+      <c r="AI112" s="85">
+        <v>14.848973875</v>
+      </c>
+      <c r="AJ112" s="86">
+        <v>14.6830883026</v>
+      </c>
+      <c r="AK112" s="86">
+        <v>0.61130994559999996</v>
+      </c>
+      <c r="AL112" s="86">
+        <v>0.85331200240000005</v>
+      </c>
+      <c r="AM112" s="86">
+        <v>0.2259587663</v>
+      </c>
+      <c r="AN112" s="86">
+        <v>30.1834506989</v>
+      </c>
+      <c r="AO112" s="86">
+        <v>7.8960964132999996</v>
+      </c>
+      <c r="AP112" s="87">
+        <v>4.7108199201999996</v>
+      </c>
+      <c r="AR112" s="85">
+        <v>15.982220010800001</v>
+      </c>
+      <c r="AS112" s="86">
+        <v>15.905175208999999</v>
+      </c>
+      <c r="AT112" s="86">
+        <v>0.77545177939999999</v>
+      </c>
+      <c r="AU112" s="86">
+        <v>0.88455660700000005</v>
+      </c>
+      <c r="AV112" s="86">
+        <v>0.21357284700000001</v>
+      </c>
+      <c r="AW112" s="86">
+        <v>19.4469280243</v>
+      </c>
+      <c r="AX112" s="86">
+        <v>4.4264597459999999</v>
+      </c>
+      <c r="AY112" s="87">
+        <v>3.3149747722999998</v>
+      </c>
+      <c r="BA112" s="85">
+        <v>22.175533294699999</v>
+      </c>
+      <c r="BB112" s="86">
+        <v>3.8634959031</v>
+      </c>
+      <c r="BC112" s="87">
+        <v>3.0084257221000001</v>
+      </c>
+      <c r="BE112" s="85">
+        <v>18.076110839799998</v>
+      </c>
+      <c r="BF112" s="86">
+        <v>3.8912318419999998</v>
+      </c>
+      <c r="BG112" s="87">
+        <v>2.8105095871999999</v>
+      </c>
+      <c r="BI112" s="85">
+        <v>15.453796386700001</v>
+      </c>
+      <c r="BJ112" s="86">
+        <v>3.3539248194</v>
+      </c>
+      <c r="BK112" s="87">
+        <v>2.4106001494</v>
+      </c>
+      <c r="BM112" s="85">
+        <v>17.437377929699998</v>
+      </c>
+      <c r="BN112" s="86">
+        <v>4.1603546348</v>
+      </c>
+      <c r="BO112" s="87">
+        <v>2.9081216274999999</v>
+      </c>
+      <c r="BQ112" s="85">
+        <v>22.608114242599999</v>
+      </c>
+      <c r="BR112" s="86">
+        <v>2.6693986912000001</v>
+      </c>
+      <c r="BS112" s="87">
+        <v>3.0097907278</v>
+      </c>
+    </row>
+    <row r="113" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A113" s="67" t="s">
+        <v>164</v>
+      </c>
       <c r="B113" s="67"/>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="67"/>
+    <row r="114" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A114" s="67" t="s">
+        <v>165</v>
+      </c>
       <c r="B114" s="67"/>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A115" s="105"/>
+    <row r="115" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A115" s="67" t="s">
+        <v>166</v>
+      </c>
       <c r="B115" s="67"/>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A116" s="105"/>
+    <row r="116" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A116" s="67" t="s">
+        <v>167</v>
+      </c>
       <c r="B116" s="67"/>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A117" s="105"/>
+    <row r="117" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A117" s="67" t="s">
+        <v>168</v>
+      </c>
       <c r="B117" s="67"/>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A118" s="106"/>
       <c r="B118" s="67"/>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" s="106"/>
+    <row r="119" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A119" s="67" t="s">
+        <v>169</v>
+      </c>
       <c r="B119" s="67"/>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A120" s="106"/>
+      <c r="Z119" s="85">
+        <v>12.021045017200001</v>
+      </c>
+      <c r="AA119" s="86">
+        <v>12.174717903099999</v>
+      </c>
+      <c r="AB119" s="86">
+        <v>0.57384321490000001</v>
+      </c>
+      <c r="AC119" s="86">
+        <v>0.80589052839999997</v>
+      </c>
+      <c r="AD119" s="86">
+        <v>0.24299263160000001</v>
+      </c>
+      <c r="AE119" s="86">
+        <v>21.576745986900001</v>
+      </c>
+      <c r="AF119" s="86">
+        <v>7.7635767836999996</v>
+      </c>
+      <c r="AG119" s="87">
+        <v>4.789752773</v>
+      </c>
+      <c r="AI119" s="85">
+        <v>14.995296506900001</v>
+      </c>
+      <c r="AJ119" s="86">
+        <v>14.813969612099999</v>
+      </c>
+      <c r="AK119" s="86">
+        <v>0.61403037520000003</v>
+      </c>
+      <c r="AL119" s="86">
+        <v>0.8620142663</v>
+      </c>
+      <c r="AM119" s="86">
+        <v>0.2203629107</v>
+      </c>
+      <c r="AN119" s="86">
+        <v>30.185325622600001</v>
+      </c>
+      <c r="AO119" s="86">
+        <v>7.8952587452999996</v>
+      </c>
+      <c r="AP119" s="87">
+        <v>4.6992112042</v>
+      </c>
+      <c r="AR119" s="85">
+        <v>16.096876525900001</v>
+      </c>
+      <c r="AS119" s="86">
+        <v>16.011472701999999</v>
+      </c>
+      <c r="AT119" s="86">
+        <v>0.7729936838</v>
+      </c>
+      <c r="AU119" s="86">
+        <v>0.88853141840000005</v>
+      </c>
+      <c r="AV119" s="86">
+        <v>0.2102357198</v>
+      </c>
+      <c r="AW119" s="86">
+        <v>19.119798660299999</v>
+      </c>
+      <c r="AX119" s="86">
+        <v>4.4199318625000004</v>
+      </c>
+      <c r="AY119" s="87">
+        <v>3.3244792110999999</v>
+      </c>
+      <c r="BA119" s="85">
+        <v>21.9029350281</v>
+      </c>
+      <c r="BB119" s="86">
+        <v>3.8874270146000001</v>
+      </c>
+      <c r="BC119" s="87">
+        <v>3.0281442703999999</v>
+      </c>
+      <c r="BE119" s="85">
+        <v>18.065368652299998</v>
+      </c>
+      <c r="BF119" s="86">
+        <v>3.9114014055999999</v>
+      </c>
+      <c r="BG119" s="87">
+        <v>2.8179561367999999</v>
+      </c>
+      <c r="BI119" s="85">
+        <v>14.9949274063</v>
+      </c>
+      <c r="BJ119" s="86">
+        <v>3.3904481759</v>
+      </c>
+      <c r="BK119" s="87">
+        <v>2.4070130839999999</v>
+      </c>
+      <c r="BM119" s="85">
+        <v>17.731140136699999</v>
+      </c>
+      <c r="BN119" s="86">
+        <v>4.1565083660999997</v>
+      </c>
+      <c r="BO119" s="87">
+        <v>2.9186445481000001</v>
+      </c>
+      <c r="BQ119" s="85">
+        <v>21.949850082400001</v>
+      </c>
+      <c r="BR119" s="86">
+        <v>2.6793967654999999</v>
+      </c>
+      <c r="BS119" s="87">
+        <v>3.012761802</v>
+      </c>
+    </row>
+    <row r="120" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A120" s="67" t="s">
+        <v>170</v>
+      </c>
       <c r="B120" s="67"/>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A121" s="106"/>
+    <row r="121" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A121" s="67" t="s">
+        <v>171</v>
+      </c>
       <c r="B121" s="67"/>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A122" s="106"/>
+    <row r="122" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A122" s="67" t="s">
+        <v>172</v>
+      </c>
       <c r="B122" s="67"/>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A123" s="106"/>
+    <row r="123" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A123" s="67" t="s">
+        <v>173</v>
+      </c>
       <c r="B123" s="67"/>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A124" s="67"/>
+    <row r="124" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A124" s="67" t="s">
+        <v>174</v>
+      </c>
       <c r="B124" s="67"/>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A125" s="68"/>
       <c r="B125" s="67"/>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A126" s="68"/>
+    <row r="126" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A126" s="67" t="s">
+        <v>175</v>
+      </c>
       <c r="B126" s="67"/>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A127" s="68"/>
+      <c r="Z126" s="85">
+        <v>12.082030550600001</v>
+      </c>
+      <c r="AA126" s="86">
+        <v>12.2337226868</v>
+      </c>
+      <c r="AB126" s="86">
+        <v>0.57761076089999996</v>
+      </c>
+      <c r="AC126" s="86">
+        <v>0.80226417380000004</v>
+      </c>
+      <c r="AD126" s="86">
+        <v>0.24642055630000001</v>
+      </c>
+      <c r="AE126" s="86">
+        <v>22.216817855799999</v>
+      </c>
+      <c r="AF126" s="86">
+        <v>7.7671568070000001</v>
+      </c>
+      <c r="AG126" s="87">
+        <v>4.7478613345999996</v>
+      </c>
+      <c r="AI126" s="85">
+        <v>15.0732185555</v>
+      </c>
+      <c r="AJ126" s="86">
+        <v>14.8837280273</v>
+      </c>
+      <c r="AK126" s="86">
+        <v>0.61713033620000002</v>
+      </c>
+      <c r="AL126" s="86">
+        <v>0.85931679009999995</v>
+      </c>
+      <c r="AM126" s="86">
+        <v>0.2249600688</v>
+      </c>
+      <c r="AN126" s="86">
+        <v>30.6709117889</v>
+      </c>
+      <c r="AO126" s="86">
+        <v>7.9225413731999996</v>
+      </c>
+      <c r="AP126" s="87">
+        <v>4.6919030400999997</v>
+      </c>
+      <c r="AR126" s="85">
+        <v>16.0763471508</v>
+      </c>
+      <c r="AS126" s="86">
+        <v>15.986009597800001</v>
+      </c>
+      <c r="AT126" s="86">
+        <v>0.77802276189999997</v>
+      </c>
+      <c r="AU126" s="86">
+        <v>0.88599557579999999</v>
+      </c>
+      <c r="AV126" s="86">
+        <v>0.21086134100000001</v>
+      </c>
+      <c r="AW126" s="86">
+        <v>19.6640281677</v>
+      </c>
+      <c r="AX126" s="86">
+        <v>4.4371174701999996</v>
+      </c>
+      <c r="AY126" s="87">
+        <v>3.3177209174</v>
+      </c>
+      <c r="BA126" s="85">
+        <v>22.602993011500001</v>
+      </c>
+      <c r="BB126" s="86">
+        <v>3.8662455131</v>
+      </c>
+      <c r="BC126" s="87">
+        <v>3.0112604269999999</v>
+      </c>
+      <c r="BE126" s="85">
+        <v>17.697351455700002</v>
+      </c>
+      <c r="BF126" s="86">
+        <v>3.9041483172999998</v>
+      </c>
+      <c r="BG126" s="87">
+        <v>2.8161654679999999</v>
+      </c>
+      <c r="BI126" s="85">
+        <v>15.3376712799</v>
+      </c>
+      <c r="BJ126" s="86">
+        <v>3.3438916500000002</v>
+      </c>
+      <c r="BK126" s="87">
+        <v>2.4130296083</v>
+      </c>
+      <c r="BM126" s="85">
+        <v>17.7614746094</v>
+      </c>
+      <c r="BN126" s="86">
+        <v>4.1570674841999997</v>
+      </c>
+      <c r="BO126" s="87">
+        <v>2.8965507346999999</v>
+      </c>
+      <c r="BQ126" s="85">
+        <v>22.790142059299999</v>
+      </c>
+      <c r="BR126" s="86">
+        <v>2.6636677594</v>
+      </c>
+      <c r="BS126" s="87">
+        <v>3.0035345376999998</v>
+      </c>
+    </row>
+    <row r="127" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A127" s="67" t="s">
+        <v>176</v>
+      </c>
       <c r="B127" s="67"/>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A128" s="69"/>
+    <row r="128" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A128" s="67" t="s">
+        <v>177</v>
+      </c>
       <c r="B128" s="67"/>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A129" s="69"/>
+    <row r="129" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A129" s="67" t="s">
+        <v>178</v>
+      </c>
       <c r="B129" s="67"/>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A130" s="69"/>
+    <row r="130" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A130" s="67" t="s">
+        <v>179</v>
+      </c>
       <c r="B130" s="67"/>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A131" s="69"/>
+    <row r="131" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A131" s="67" t="s">
+        <v>180</v>
+      </c>
       <c r="B131" s="67"/>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:71" x14ac:dyDescent="0.2">
       <c r="A132" s="69"/>
       <c r="B132" s="67"/>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A133" s="67"/>
+    <row r="133" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A133" s="67" t="s">
+        <v>181</v>
+      </c>
       <c r="B133" s="67"/>
+      <c r="Z133" s="85">
+        <v>11.943336327900001</v>
+      </c>
+      <c r="AA133" s="86">
+        <v>12.0726165771</v>
+      </c>
+      <c r="AB133" s="86">
+        <v>0.570239685</v>
+      </c>
+      <c r="AC133" s="86">
+        <v>0.80173936290000003</v>
+      </c>
+      <c r="AD133" s="86">
+        <v>0.24727641</v>
+      </c>
+      <c r="AE133" s="86">
+        <v>21.298913955700002</v>
+      </c>
+      <c r="AF133" s="86">
+        <v>7.7404890463999996</v>
+      </c>
+      <c r="AG133" s="87">
+        <v>4.8081665666999998</v>
+      </c>
+      <c r="AI133" s="85">
+        <v>14.905336351400001</v>
+      </c>
+      <c r="AJ133" s="86">
+        <v>14.701739311200001</v>
+      </c>
+      <c r="AK133" s="86">
+        <v>0.61115875419999999</v>
+      </c>
+      <c r="AL133" s="86">
+        <v>0.859180426</v>
+      </c>
+      <c r="AM133" s="86">
+        <v>0.2238106433</v>
+      </c>
+      <c r="AN133" s="86">
+        <v>29.916112899800002</v>
+      </c>
+      <c r="AO133" s="86">
+        <v>7.8849444749000002</v>
+      </c>
+      <c r="AP133" s="87">
+        <v>4.7106583420000003</v>
+      </c>
+      <c r="AR133" s="85">
+        <v>15.9865535736</v>
+      </c>
+      <c r="AS133" s="86">
+        <v>15.889166832000001</v>
+      </c>
+      <c r="AT133" s="86">
+        <v>0.77214431760000002</v>
+      </c>
+      <c r="AU133" s="86">
+        <v>0.88535752300000004</v>
+      </c>
+      <c r="AV133" s="86">
+        <v>0.21608437599999999</v>
+      </c>
+      <c r="AW133" s="86">
+        <v>19.187402725199998</v>
+      </c>
+      <c r="AX133" s="86">
+        <v>4.4154131136999997</v>
+      </c>
+      <c r="AY133" s="87">
+        <v>3.3198028032</v>
+      </c>
+      <c r="BA133" s="85">
+        <v>21.876766204799999</v>
+      </c>
+      <c r="BB133" s="86">
+        <v>3.8593273789000002</v>
+      </c>
+      <c r="BC133" s="87">
+        <v>3.0153362543000002</v>
+      </c>
+      <c r="BE133" s="85">
+        <v>17.657897949199999</v>
+      </c>
+      <c r="BF133" s="86">
+        <v>3.8837025762000001</v>
+      </c>
+      <c r="BG133" s="87">
+        <v>2.8121074867</v>
+      </c>
+      <c r="BI133" s="85">
+        <v>15.0709266663</v>
+      </c>
+      <c r="BJ133" s="86">
+        <v>3.3681001014</v>
+      </c>
+      <c r="BK133" s="87">
+        <v>2.4065245965000002</v>
+      </c>
+      <c r="BM133" s="85">
+        <v>17.914672851599999</v>
+      </c>
+      <c r="BN133" s="86">
+        <v>4.1924394867999997</v>
+      </c>
+      <c r="BO133" s="87">
+        <v>2.8858418363</v>
+      </c>
+      <c r="BQ133" s="85">
+        <v>22.653158187900001</v>
+      </c>
+      <c r="BR133" s="86">
+        <v>2.6656925791999999</v>
+      </c>
+      <c r="BS133" s="87">
+        <v>3.0126918835000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A134" s="67" t="s">
+        <v>182</v>
+      </c>
+      <c r="B134" s="67"/>
+    </row>
+    <row r="135" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A135" s="67" t="s">
+        <v>183</v>
+      </c>
+      <c r="B135" s="115"/>
+    </row>
+    <row r="136" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A136" s="67" t="s">
+        <v>184</v>
+      </c>
+      <c r="B136" s="115"/>
+    </row>
+    <row r="137" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A137" s="67" t="s">
+        <v>185</v>
+      </c>
+      <c r="B137" s="115"/>
+    </row>
+    <row r="138" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A138" s="67" t="s">
+        <v>186</v>
+      </c>
+      <c r="B138" s="115"/>
+    </row>
+    <row r="139" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A139" s="69"/>
+      <c r="B139" s="115"/>
+    </row>
+    <row r="140" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A140" s="67" t="s">
+        <v>187</v>
+      </c>
+      <c r="B140" s="115"/>
+      <c r="Z140" s="85">
+        <v>11.925304095</v>
+      </c>
+      <c r="AA140" s="86">
+        <v>12.070079803500001</v>
+      </c>
+      <c r="AB140" s="86">
+        <v>0.5697257201</v>
+      </c>
+      <c r="AC140" s="86">
+        <v>0.80080055000000006</v>
+      </c>
+      <c r="AD140" s="86">
+        <v>0.24584487969999999</v>
+      </c>
+      <c r="AE140" s="86">
+        <v>21.414442062399999</v>
+      </c>
+      <c r="AF140" s="86">
+        <v>7.7729569081000003</v>
+      </c>
+      <c r="AG140" s="87">
+        <v>4.8014497299999999</v>
+      </c>
+      <c r="AI140" s="85">
+        <v>14.8718429804</v>
+      </c>
+      <c r="AJ140" s="86">
+        <v>14.6909713745</v>
+      </c>
+      <c r="AK140" s="86">
+        <v>0.61079539810000005</v>
+      </c>
+      <c r="AL140" s="86">
+        <v>0.8582474524</v>
+      </c>
+      <c r="AM140" s="86">
+        <v>0.2229632768</v>
+      </c>
+      <c r="AN140" s="86">
+        <v>29.905317306499999</v>
+      </c>
+      <c r="AO140" s="86">
+        <v>7.8817443811999999</v>
+      </c>
+      <c r="AP140" s="87">
+        <v>4.707540388</v>
+      </c>
+      <c r="AR140" s="85">
+        <v>15.979407892199999</v>
+      </c>
+      <c r="AS140" s="86">
+        <v>15.887923240699999</v>
+      </c>
+      <c r="AT140" s="86">
+        <v>0.77118149849999995</v>
+      </c>
+      <c r="AU140" s="86">
+        <v>0.88547287699999999</v>
+      </c>
+      <c r="AV140" s="86">
+        <v>0.2114117147</v>
+      </c>
+      <c r="AW140" s="86">
+        <v>19.2417678833</v>
+      </c>
+      <c r="AX140" s="86">
+        <v>4.4225783528999996</v>
+      </c>
+      <c r="AY140" s="87">
+        <v>3.3107491843000001</v>
+      </c>
+      <c r="BA140" s="85">
+        <v>22.167385101299999</v>
+      </c>
+      <c r="BB140" s="86">
+        <v>3.8527710144</v>
+      </c>
+      <c r="BC140" s="87">
+        <v>3.0074305334</v>
+      </c>
+      <c r="BE140" s="85">
+        <v>18.143201827999999</v>
+      </c>
+      <c r="BF140" s="86">
+        <v>3.9212541283000002</v>
+      </c>
+      <c r="BG140" s="87">
+        <v>2.8180496539000002</v>
+      </c>
+      <c r="BI140" s="85">
+        <v>15.307800293</v>
+      </c>
+      <c r="BJ140" s="86">
+        <v>3.3756711680999998</v>
+      </c>
+      <c r="BK140" s="87">
+        <v>2.4148324582999998</v>
+      </c>
+      <c r="BM140" s="85">
+        <v>17.7208862305</v>
+      </c>
+      <c r="BN140" s="86">
+        <v>4.1613274122000004</v>
+      </c>
+      <c r="BO140" s="87">
+        <v>2.8892014121999998</v>
+      </c>
+      <c r="BQ140" s="85">
+        <v>22.478149414099999</v>
+      </c>
+      <c r="BR140" s="86">
+        <v>2.6611728765999998</v>
+      </c>
+      <c r="BS140" s="87">
+        <v>3.0151470593999998</v>
+      </c>
+    </row>
+    <row r="141" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A141" s="67" t="s">
+        <v>188</v>
+      </c>
+      <c r="B141" s="67"/>
+    </row>
+    <row r="142" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A142" s="67" t="s">
+        <v>189</v>
+      </c>
+      <c r="B142" s="115"/>
+    </row>
+    <row r="143" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A143" s="67" t="s">
+        <v>190</v>
+      </c>
+      <c r="B143" s="115"/>
+    </row>
+    <row r="144" spans="1:71" x14ac:dyDescent="0.2">
+      <c r="A144" s="67" t="s">
+        <v>191</v>
+      </c>
+      <c r="B144" s="115"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A145" s="67" t="s">
+        <v>192</v>
+      </c>
+      <c r="B145" s="115"/>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A146" s="69"/>
+      <c r="B146" s="115"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>